<commit_message>
take away notes updated
</commit_message>
<xml_diff>
--- a/take_aways.xlsx
+++ b/take_aways.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nithesh\Documents\github\CP_notes\CP_notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4380D207-FDD2-491F-84F7-60BAA9C95DAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDAA992A-E5DB-4355-9F9D-B91C8D185CED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A1066A7A-5E28-47FA-AFBA-961FD32DAE58}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="44">
   <si>
     <t>problem</t>
   </si>
@@ -154,6 +154,18 @@
   </si>
   <si>
     <t>One thing I noticed is  I am sometimes while thinking thru my ideas. for some reason I give up my ideas half way even tho if I write it down and do full analyze it once I might get the answer don’t visualize logic and leave it am not at that level to do without pen paper use it for now</t>
+  </si>
+  <si>
+    <t>https://codeforces.com/problemset/problem/2002/C</t>
+  </si>
+  <si>
+    <t>cf 1200</t>
+  </si>
+  <si>
+    <t>looked very hard in the start but had sweet maths solution to it</t>
+  </si>
+  <si>
+    <t>do not convert numbers into decimal will loose precision so try to keep it as whole numbers in any comparison if possible change equation of conversion from division to multiplication</t>
   </si>
 </sst>
 </file>
@@ -522,10 +534,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F36718C-7E11-4E10-92EF-1CA1F277B1DA}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -730,6 +742,23 @@
         <v>39</v>
       </c>
     </row>
+    <row r="11" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="B11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{07866BBE-2668-48A8-96D1-A68747CEBA01}"/>

</xml_diff>

<commit_message>
take_away updated and bitwise formula added
</commit_message>
<xml_diff>
--- a/take_aways.xlsx
+++ b/take_aways.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nithesh\Documents\github\CP_notes\CP_notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99D32EA0-A5A3-411B-8CA1-CB2F9BB076CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9585F99-E651-4B52-A980-1AE4538D29C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A1066A7A-5E28-47FA-AFBA-961FD32DAE58}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="87">
   <si>
     <t>problem</t>
   </si>
@@ -286,6 +286,15 @@
   </si>
   <si>
     <t xml:space="preserve">gcd(x, x + 1) == 1 </t>
+  </si>
+  <si>
+    <t>https://codeforces.com/contest/2085/problem/C</t>
+  </si>
+  <si>
+    <t>cf 1600</t>
+  </si>
+  <si>
+    <t>some imp bitwise equations : https://codeforces.com/blog/entry/94470</t>
   </si>
 </sst>
 </file>
@@ -654,10 +663,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F36718C-7E11-4E10-92EF-1CA1F277B1DA}">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1064,6 +1073,20 @@
         <v>83</v>
       </c>
     </row>
+    <row r="25" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B25" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{07866BBE-2668-48A8-96D1-A68747CEBA01}"/>

</xml_diff>